<commit_message>
Commit after add System1_Open, System1_Close
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13035" windowHeight="8145"/>
+    <workbookView windowWidth="13035" windowHeight="7560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -151,12 +151,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -166,7 +160,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -201,6 +195,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -208,9 +227,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -223,11 +256,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -246,67 +301,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -317,19 +311,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -341,37 +347,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -383,31 +359,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -425,7 +377,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,7 +389,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -449,13 +413,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -467,19 +443,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -491,13 +467,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -514,8 +508,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -523,8 +517,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -544,17 +553,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -566,30 +564,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -608,165 +582,181 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1088,7 +1078,7 @@
   <sheetPr/>
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -1135,13 +1125,13 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" ht="14.25" customHeight="1" spans="1:3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1152,7 +1142,7 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1160,7 +1150,7 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2178,8 +2168,8 @@
   <sheetPr/>
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -2229,7 +2219,7 @@
         <v>13</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>14</v>

</xml_diff>